<commit_message>
added questionnaire and pricing group to RD to import made language, country, currency and province upper case all the time added a import hs tab for hubspot, with its headers subset as requested by Ben
</commit_message>
<xml_diff>
--- a/hiring_client_input_template.xlsx
+++ b/hiring_client_input_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slavigne\PycharmProjects\icm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\armeunier\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E256AE-1A99-40E0-898F-C71203F72B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A66669-2B12-4B30-BEA9-30CC15AEC2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="2200" windowWidth="28800" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="list" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="799">
   <si>
     <t>city</t>
   </si>
@@ -2320,13 +2320,142 @@
   <si>
     <t>patheon</t>
   </si>
+  <si>
+    <t>GD_Valleyfield</t>
+  </si>
+  <si>
+    <t>gouvernance_au_feminin_national</t>
+  </si>
+  <si>
+    <t>gouvernance_au_feminin_international</t>
+  </si>
+  <si>
+    <t>bell</t>
+  </si>
+  <si>
+    <t>carrier</t>
+  </si>
+  <si>
+    <t>elearning</t>
+  </si>
+  <si>
+    <t>portail_pfr</t>
+  </si>
+  <si>
+    <t>special_19</t>
+  </si>
+  <si>
+    <t>covid_extension_1</t>
+  </si>
+  <si>
+    <t>covid_extension_2</t>
+  </si>
+  <si>
+    <t>covid_extension_3</t>
+  </si>
+  <si>
+    <t>low_risk</t>
+  </si>
+  <si>
+    <t>retention</t>
+  </si>
+  <si>
+    <t>back_to_work</t>
+  </si>
+  <si>
+    <t>rbm_rio_tinto</t>
+  </si>
+  <si>
+    <t>crh</t>
+  </si>
+  <si>
+    <t>special_flat_rate_780</t>
+  </si>
+  <si>
+    <t>pratt</t>
+  </si>
+  <si>
+    <t>cae_temp_372</t>
+  </si>
+  <si>
+    <t>cae_temp_434</t>
+  </si>
+  <si>
+    <t>cae_temp_496</t>
+  </si>
+  <si>
+    <t>cae_temp_558</t>
+  </si>
+  <si>
+    <t>third_party</t>
+  </si>
+  <si>
+    <t>caetemp1</t>
+  </si>
+  <si>
+    <t>caetemp2</t>
+  </si>
+  <si>
+    <t>Metro_Niveau_1</t>
+  </si>
+  <si>
+    <t>Metro_Niveau_2</t>
+  </si>
+  <si>
+    <t>Metro_Niveau_3</t>
+  </si>
+  <si>
+    <t>old_standard</t>
+  </si>
+  <si>
+    <t>rta</t>
+  </si>
+  <si>
+    <t>per_country</t>
+  </si>
+  <si>
+    <t>cae_280</t>
+  </si>
+  <si>
+    <t>Exxon_Mobil</t>
+  </si>
+  <si>
+    <t>Metro_Niveau_1_Standard</t>
+  </si>
+  <si>
+    <t>Metro_Niveau_2_Standard</t>
+  </si>
+  <si>
+    <t>Metro_Niveau_3_Standard</t>
+  </si>
+  <si>
+    <t>Imerys</t>
+  </si>
+  <si>
+    <t>Hydro_Québec_0_5employees</t>
+  </si>
+  <si>
+    <t>Hydro_Québec_6_19_employees</t>
+  </si>
+  <si>
+    <t>Hydro_Québec_20_99_employees</t>
+  </si>
+  <si>
+    <t>Hydro_Québec100_499_employees</t>
+  </si>
+  <si>
+    <t>Hydro_Québec_500_et_plus_employees</t>
+  </si>
+  <si>
+    <t>Tahiti</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
@@ -3017,9 +3146,9 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -3069,8 +3198,14 @@
     <xf numFmtId="14" fontId="0" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="44" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="44" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="42" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3120,246 +3255,6 @@
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="38">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -3470,6 +3365,246 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3489,60 +3624,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FE76ACF-87D2-4B37-A2A4-5B978799C529}" name="Table1" displayName="Table1" ref="A1:AQ3000" totalsRowShown="0" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FE76ACF-87D2-4B37-A2A4-5B978799C529}" name="Table1" displayName="Table1" ref="A1:AQ3000" totalsRowShown="0" headerRowDxfId="37">
   <autoFilter ref="A1:AQ3000" xr:uid="{2FE76ACF-87D2-4B37-A2A4-5B978799C529}"/>
   <tableColumns count="43">
     <tableColumn id="1" xr3:uid="{68B0E6D0-1768-41A0-A52B-C828170AB410}" name="contractor_name"/>
     <tableColumn id="2" xr3:uid="{C2CCD438-C358-4B31-BED4-353DE5DB93C2}" name="contact_first_name"/>
-    <tableColumn id="3" xr3:uid="{09230401-9549-4B0B-AC7D-F36C0B202C28}" name="contact_last_name" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{09230401-9549-4B0B-AC7D-F36C0B202C28}" name="contact_last_name" dataDxfId="36"/>
     <tableColumn id="4" xr3:uid="{FACD9BBB-E590-4BDC-81EE-B17802D44CEC}" name="contact_email"/>
     <tableColumn id="5" xr3:uid="{8DEFE57A-D03B-471D-BFCE-3D05A7A52CC8}" name="contact_phone"/>
     <tableColumn id="6" xr3:uid="{C7ED889A-5671-4F18-8380-099F4D716044}" name="contact_language"/>
-    <tableColumn id="7" xr3:uid="{9423739C-A9C4-4673-849B-BD582AD0209B}" name="address" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{9423739C-A9C4-4673-849B-BD582AD0209B}" name="address" dataDxfId="35"/>
     <tableColumn id="8" xr3:uid="{CDB1BF20-1A5E-4253-9BA0-214DC802B4BE}" name="city"/>
     <tableColumn id="9" xr3:uid="{B544AD04-CCB4-4EA3-B419-09B6136558E7}" name="province_state_iso2"/>
     <tableColumn id="10" xr3:uid="{DD89521D-4F42-4297-B202-D3BF2F8C3F49}" name="country_iso2"/>
     <tableColumn id="11" xr3:uid="{8AF8A3F8-8D83-4663-BA45-7AB3EADD9F50}" name="postal_code"/>
     <tableColumn id="12" xr3:uid="{31258067-2CB8-4C32-BFD2-9F35DF2E1B38}" name="category"/>
     <tableColumn id="36" xr3:uid="{9E9C639C-5ADB-4397-AF44-99E7CDDEA131}" name="description"/>
-    <tableColumn id="40" xr3:uid="{602B1E66-862D-4FA0-881B-D68E6D722BAD}" name="phone" dataDxfId="1"/>
-    <tableColumn id="41" xr3:uid="{22BAA284-8A8B-411D-846D-FCC48FD9226C}" name="extension" dataDxfId="0"/>
+    <tableColumn id="40" xr3:uid="{602B1E66-862D-4FA0-881B-D68E6D722BAD}" name="phone" dataDxfId="34"/>
+    <tableColumn id="41" xr3:uid="{22BAA284-8A8B-411D-846D-FCC48FD9226C}" name="extension" dataDxfId="33"/>
     <tableColumn id="31" xr3:uid="{B5DC8495-BE6F-4F7C-86F9-CEAB39AB3247}" name="fax"/>
     <tableColumn id="38" xr3:uid="{9088F168-874C-4AE3-B9A8-89D690F57343}" name="website"/>
-    <tableColumn id="42" xr3:uid="{D981BE1D-9D97-4040-AC33-95DA063ECFB7}" name="language" dataDxfId="23">
+    <tableColumn id="42" xr3:uid="{D981BE1D-9D97-4040-AC33-95DA063ECFB7}" name="language" dataDxfId="32">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[contact_language]]),"",Table1[[#This Row],[contact_language]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{5A93FE27-69F3-452F-834A-DEEE27494DD3}" name="is_take_over" dataDxfId="22">
+    <tableColumn id="13" xr3:uid="{5A93FE27-69F3-452F-834A-DEEE27494DD3}" name="is_take_over" dataDxfId="31">
       <calculatedColumnFormula>IF(NOT(ISBLANK(Table1[[#This Row],[qualification_status]])),TRUE,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{71CD9A9A-B28D-494B-8B05-3CB38B83218E}" name="qualification_expiration_date" dataDxfId="21">
+    <tableColumn id="14" xr3:uid="{71CD9A9A-B28D-494B-8B05-3CB38B83218E}" name="qualification_expiration_date" dataDxfId="30">
       <calculatedColumnFormula>2022/1/1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{D3D87C07-9251-492A-B655-E40DEA0C6DBC}" name="qualification_status"/>
-    <tableColumn id="16" xr3:uid="{E75BD467-D145-4908-BFC4-38521658C094}" name="batch" dataDxfId="20"/>
-    <tableColumn id="17" xr3:uid="{7FA6C153-F27E-4A9A-AA8B-F1724C785F5F}" name="questionnaire_name" dataDxfId="19"/>
-    <tableColumn id="18" xr3:uid="{92064B28-FD31-46AA-B7C1-5EC6329CF5B9}" name="questionnaire_id" dataDxfId="18"/>
-    <tableColumn id="39" xr3:uid="{9E81AE14-E64D-4F9F-89B5-6F46228C6ABA}" name="pricing_group_id" dataDxfId="17"/>
-    <tableColumn id="19" xr3:uid="{3C35D03C-6D0C-4958-A56A-C70985B40274}" name="pricing_group_code" dataDxfId="16"/>
-    <tableColumn id="20" xr3:uid="{27F05B6B-229E-4F32-9E3C-DAD9AEA1AD54}" name="hiring_client_name" dataDxfId="15"/>
-    <tableColumn id="21" xr3:uid="{90735E31-A872-4DF4-9027-4E0DAC6A62E3}" name="hiring_client_id" dataDxfId="14"/>
-    <tableColumn id="22" xr3:uid="{5505DCB2-B613-4EFA-B9E9-90209ED148C3}" name="is_association_fee" dataDxfId="13"/>
-    <tableColumn id="23" xr3:uid="{96E69634-021C-4770-9F72-686A4478222D}" name="base_subscription_fee" dataDxfId="12" dataCellStyle="Currency"/>
-    <tableColumn id="35" xr3:uid="{404BF0A1-D64E-4EAE-91AE-D8F26AB31B3B}" name="contact_currency" dataDxfId="11"/>
-    <tableColumn id="34" xr3:uid="{F85216EA-CAC8-47DE-97F8-F1AE4E8DEBF4}" name="agent_in_charge_id" dataDxfId="10"/>
-    <tableColumn id="32" xr3:uid="{34FEC987-EE56-4BE3-9A28-B87F778878E2}" name="take_over_follow-up_date" dataDxfId="9"/>
-    <tableColumn id="43" xr3:uid="{24E6A6B9-19FC-4E13-B14E-B590935FD4F6}" name="renewal_date" dataDxfId="8">
+    <tableColumn id="16" xr3:uid="{E75BD467-D145-4908-BFC4-38521658C094}" name="batch" dataDxfId="29"/>
+    <tableColumn id="17" xr3:uid="{7FA6C153-F27E-4A9A-AA8B-F1724C785F5F}" name="questionnaire_name" dataDxfId="28"/>
+    <tableColumn id="18" xr3:uid="{92064B28-FD31-46AA-B7C1-5EC6329CF5B9}" name="questionnaire_id" dataDxfId="27"/>
+    <tableColumn id="39" xr3:uid="{9E81AE14-E64D-4F9F-89B5-6F46228C6ABA}" name="pricing_group_id" dataDxfId="26"/>
+    <tableColumn id="19" xr3:uid="{3C35D03C-6D0C-4958-A56A-C70985B40274}" name="pricing_group_code" dataDxfId="25"/>
+    <tableColumn id="20" xr3:uid="{27F05B6B-229E-4F32-9E3C-DAD9AEA1AD54}" name="hiring_client_name" dataDxfId="24"/>
+    <tableColumn id="21" xr3:uid="{90735E31-A872-4DF4-9027-4E0DAC6A62E3}" name="hiring_client_id" dataDxfId="23"/>
+    <tableColumn id="22" xr3:uid="{5505DCB2-B613-4EFA-B9E9-90209ED148C3}" name="is_association_fee" dataDxfId="22"/>
+    <tableColumn id="23" xr3:uid="{96E69634-021C-4770-9F72-686A4478222D}" name="base_subscription_fee" dataDxfId="21" dataCellStyle="Currency"/>
+    <tableColumn id="35" xr3:uid="{404BF0A1-D64E-4EAE-91AE-D8F26AB31B3B}" name="contact_currency" dataDxfId="20"/>
+    <tableColumn id="34" xr3:uid="{F85216EA-CAC8-47DE-97F8-F1AE4E8DEBF4}" name="agent_in_charge_id" dataDxfId="19"/>
+    <tableColumn id="32" xr3:uid="{34FEC987-EE56-4BE3-9A28-B87F778878E2}" name="take_over_follow-up_date" dataDxfId="18"/>
+    <tableColumn id="43" xr3:uid="{24E6A6B9-19FC-4E13-B14E-B590935FD4F6}" name="renewal_date" dataDxfId="17">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[qualification_expiration_date]]),"",Table1[[#This Row],[qualification_expiration_date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{17293FBA-9443-4065-8F86-4F7218EA94D6}" name="information_shared" dataDxfId="7"/>
-    <tableColumn id="33" xr3:uid="{FC707AB8-53E5-404D-897E-524F17A56A4A}" name="contact_timezone" dataDxfId="6"/>
-    <tableColumn id="24" xr3:uid="{13D6A045-4C18-4A0E-982B-198DCCFF4AF6}" name="do_not_match" dataDxfId="5"/>
-    <tableColumn id="25" xr3:uid="{56679A03-B0BC-48AB-AF15-3AE6D5F461CE}" name="force_cbx_id" dataDxfId="4"/>
-    <tableColumn id="26" xr3:uid="{44631EFC-C0D2-489B-9224-008144E39C83}" name="ambiguous" dataDxfId="3"/>
+    <tableColumn id="37" xr3:uid="{17293FBA-9443-4065-8F86-4F7218EA94D6}" name="information_shared" dataDxfId="16"/>
+    <tableColumn id="33" xr3:uid="{FC707AB8-53E5-404D-897E-524F17A56A4A}" name="contact_timezone" dataDxfId="15"/>
+    <tableColumn id="24" xr3:uid="{13D6A045-4C18-4A0E-982B-198DCCFF4AF6}" name="do_not_match" dataDxfId="14"/>
+    <tableColumn id="25" xr3:uid="{56679A03-B0BC-48AB-AF15-3AE6D5F461CE}" name="force_cbx_id" dataDxfId="13"/>
+    <tableColumn id="26" xr3:uid="{44631EFC-C0D2-489B-9224-008144E39C83}" name="ambiguous" dataDxfId="12"/>
     <tableColumn id="27" xr3:uid="{95EAFCA8-990A-4A3A-9C7C-2D1C4DA52F98}" name="metadata[_cm|_gm|_rm]_x"/>
     <tableColumn id="30" xr3:uid="{8EB8B163-6333-444D-9E65-8880DB3F12A0}" name="metadata[_cm|_gm|_rm]_y"/>
     <tableColumn id="28" xr3:uid="{534D7E5E-F672-4254-9991-B364A870A48C}" name="metadata[_cm|_gm|_rm]_z"/>
-    <tableColumn id="29" xr3:uid="{E37FE82A-F5C7-47D6-82C6-4BBC3EF97AD9}" name="metadata[_cm|_gm|_rm]_zz" dataDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{E37FE82A-F5C7-47D6-82C6-4BBC3EF97AD9}" name="metadata[_cm|_gm|_rm]_zz" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3847,8 +3982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ3000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N3006" sqref="N3006"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -49606,53 +49741,53 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J2:J3000">
-    <cfRule type="expression" dxfId="37" priority="10">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>IF(ISBLANK($J2),FALSE,NOT(COUNTIF(Countries,$J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F3000">
-    <cfRule type="expression" dxfId="36" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>IF(ISBLANK($F2),FALSE,NOT(COUNTIF(Languages,$F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE2:AE3000">
-    <cfRule type="expression" dxfId="35" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>IF(ISBLANK(AE2),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>IF(ISBLANK($AE2),FALSE,IF(AND($AE2="CAD",$J2="CA"),FALSE,IF(AND($AE2&lt;&gt;"CAD",$J2="CA"),TRUE,IF($AE2="USD",FALSE,TRUE))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="11">
+    <cfRule type="expression" dxfId="6" priority="11">
       <formula>IF(ISBLANK($AE2),FALSE,NOT(COUNTIF(Currencies,$AE2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U3000">
-    <cfRule type="expression" dxfId="32" priority="8">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>IF(ISBLANK($U2),FALSE,NOT(COUNTIF(QualificationStatus,$U2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ2:AJ3000">
-    <cfRule type="expression" dxfId="31" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>IF(ISBLANK($AJ2),FALSE,NOT(COUNTIF(Timezones,$AJ2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I3000">
-    <cfRule type="expression" dxfId="30" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>IF(ISBLANK($I2),FALSE,IF($J2="CA",NOT(COUNTIF(ProvincesCA,$I2)),IF($J2="US",NOT(COUNTIF(ProvincesUS,$I2)),FALSE)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:K3000">
-    <cfRule type="expression" dxfId="29" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>IF(ISBLANK(A2),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI2:AJ3000">
-    <cfRule type="expression" dxfId="28" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>IF(ISBLANK(AI2),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI2:AI3000">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>IF(ISBLANK($AI2),FALSE,NOT(COUNTIF(YesNo,$AI2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -49702,8 +49837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B287471-A9B4-4B6A-92DB-2DB011DD2C9B}">
   <dimension ref="A1:R295"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -49724,7 +49859,7 @@
     <col min="15" max="15" width="10.1796875" style="20" customWidth="1"/>
     <col min="16" max="16" width="39.453125" style="20" customWidth="1"/>
     <col min="17" max="17" width="14.90625" style="20" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.36328125" style="20" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.90625" style="20" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="27.1796875" style="20" customWidth="1"/>
     <col min="20" max="16384" width="12.54296875" style="20"/>
   </cols>
@@ -49814,10 +49949,10 @@
       <c r="P2" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="Q2" s="20">
+      <c r="Q2" s="47">
         <v>1</v>
       </c>
-      <c r="R2" s="20" t="s">
+      <c r="R2" s="17" t="s">
         <v>748</v>
       </c>
     </row>
@@ -49864,10 +49999,10 @@
       <c r="P3" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="Q3" s="20">
+      <c r="Q3" s="47">
         <v>2</v>
       </c>
-      <c r="R3" s="20" t="s">
+      <c r="R3" s="17" t="s">
         <v>749</v>
       </c>
     </row>
@@ -49911,10 +50046,10 @@
       <c r="P4" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="Q4" s="20">
+      <c r="Q4" s="47">
         <v>3</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="R4" s="17" t="s">
         <v>750</v>
       </c>
     </row>
@@ -49955,10 +50090,10 @@
         <v>101</v>
       </c>
       <c r="N5" s="22"/>
-      <c r="Q5" s="20">
+      <c r="Q5" s="47">
         <v>4</v>
       </c>
-      <c r="R5" s="20" t="s">
+      <c r="R5" s="17" t="s">
         <v>751</v>
       </c>
     </row>
@@ -49993,10 +50128,10 @@
         <v>110</v>
       </c>
       <c r="N6" s="22"/>
-      <c r="Q6" s="20">
+      <c r="Q6" s="47">
         <v>5</v>
       </c>
-      <c r="R6" s="20" t="s">
+      <c r="R6" s="17" t="s">
         <v>752</v>
       </c>
     </row>
@@ -50031,10 +50166,10 @@
         <v>119</v>
       </c>
       <c r="N7" s="22"/>
-      <c r="Q7" s="20">
+      <c r="Q7" s="47">
         <v>6</v>
       </c>
-      <c r="R7" s="20" t="s">
+      <c r="R7" s="17" t="s">
         <v>753</v>
       </c>
     </row>
@@ -50066,10 +50201,10 @@
         <v>126</v>
       </c>
       <c r="N8" s="22"/>
-      <c r="Q8" s="20">
+      <c r="Q8" s="47">
         <v>7</v>
       </c>
-      <c r="R8" s="20" t="s">
+      <c r="R8" s="17" t="s">
         <v>754</v>
       </c>
     </row>
@@ -50095,10 +50230,10 @@
         <v>131</v>
       </c>
       <c r="N9" s="22"/>
-      <c r="Q9" s="20">
+      <c r="Q9" s="47">
         <v>8</v>
       </c>
-      <c r="R9" s="20" t="s">
+      <c r="R9" s="17" t="s">
         <v>755</v>
       </c>
     </row>
@@ -50124,6 +50259,12 @@
         <v>136</v>
       </c>
       <c r="N10" s="22"/>
+      <c r="Q10" s="47">
+        <v>9</v>
+      </c>
+      <c r="R10" s="17" t="s">
+        <v>757</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C11" s="20" t="s">
@@ -50147,6 +50288,12 @@
         <v>141</v>
       </c>
       <c r="N11" s="22"/>
+      <c r="Q11" s="47">
+        <v>10</v>
+      </c>
+      <c r="R11" s="17" t="s">
+        <v>758</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C12" s="20" t="s">
@@ -50170,6 +50317,12 @@
         <v>146</v>
       </c>
       <c r="N12" s="22"/>
+      <c r="Q12" s="47">
+        <v>14</v>
+      </c>
+      <c r="R12" s="17" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C13" s="20" t="s">
@@ -50193,6 +50346,12 @@
         <v>152</v>
       </c>
       <c r="N13" s="22"/>
+      <c r="Q13" s="47">
+        <v>15</v>
+      </c>
+      <c r="R13" s="17" t="s">
+        <v>760</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C14" s="20" t="s">
@@ -50216,6 +50375,12 @@
         <v>157</v>
       </c>
       <c r="N14" s="22"/>
+      <c r="Q14" s="47">
+        <v>16</v>
+      </c>
+      <c r="R14" s="17" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C15" s="20" t="s">
@@ -50235,6 +50400,12 @@
       <c r="L15" s="22"/>
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
+      <c r="Q15" s="47">
+        <v>17</v>
+      </c>
+      <c r="R15" s="17" t="s">
+        <v>762</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C16" s="20" t="s">
@@ -50260,8 +50431,14 @@
         <v>76</v>
       </c>
       <c r="N16" s="22"/>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q16" s="47">
+        <v>18</v>
+      </c>
+      <c r="R16" s="17" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C17" s="20" t="s">
         <v>147</v>
       </c>
@@ -50283,8 +50460,14 @@
         <v>168</v>
       </c>
       <c r="N17" s="22"/>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q17" s="47">
+        <v>19</v>
+      </c>
+      <c r="R17" s="17" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C18" s="20" t="s">
         <v>169</v>
       </c>
@@ -50306,8 +50489,14 @@
         <v>155</v>
       </c>
       <c r="N18" s="22"/>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q18" s="47">
+        <v>20</v>
+      </c>
+      <c r="R18" s="17" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C19" s="20" t="s">
         <v>169</v>
       </c>
@@ -50329,8 +50518,14 @@
         <v>129</v>
       </c>
       <c r="N19" s="22"/>
-    </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q19" s="47">
+        <v>21</v>
+      </c>
+      <c r="R19" s="17" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C20" s="20" t="s">
         <v>169</v>
       </c>
@@ -50352,8 +50547,14 @@
         <v>37</v>
       </c>
       <c r="N20" s="22"/>
-    </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q20" s="47">
+        <v>22</v>
+      </c>
+      <c r="R20" s="17" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="21" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C21" s="20" t="s">
         <v>169</v>
       </c>
@@ -50375,8 +50576,14 @@
         <v>185</v>
       </c>
       <c r="N21" s="22"/>
-    </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q21" s="47">
+        <v>24</v>
+      </c>
+      <c r="R21" s="17" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="22" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C22" s="20" t="s">
         <v>186</v>
       </c>
@@ -50398,8 +50605,14 @@
         <v>191</v>
       </c>
       <c r="N22" s="22"/>
-    </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q22" s="47">
+        <v>25</v>
+      </c>
+      <c r="R22" s="17" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C23" s="20" t="s">
         <v>186</v>
       </c>
@@ -50421,8 +50634,14 @@
         <v>196</v>
       </c>
       <c r="N23" s="22"/>
-    </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q23" s="47">
+        <v>26</v>
+      </c>
+      <c r="R23" s="17" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C24" s="20" t="s">
         <v>186</v>
       </c>
@@ -50444,8 +50663,14 @@
         <v>201</v>
       </c>
       <c r="N24" s="22"/>
-    </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q24" s="47">
+        <v>27</v>
+      </c>
+      <c r="R24" s="17" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C25" s="20" t="s">
         <v>186</v>
       </c>
@@ -50467,8 +50692,14 @@
         <v>206</v>
       </c>
       <c r="N25" s="22"/>
-    </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q25" s="47">
+        <v>28</v>
+      </c>
+      <c r="R25" s="17" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C26" s="20" t="s">
         <v>207</v>
       </c>
@@ -50490,8 +50721,14 @@
         <v>211</v>
       </c>
       <c r="N26" s="22"/>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q26" s="47">
+        <v>29</v>
+      </c>
+      <c r="R26" s="17" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C27" s="20" t="s">
         <v>212</v>
       </c>
@@ -50513,8 +50750,14 @@
         <v>217</v>
       </c>
       <c r="N27" s="22"/>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q27" s="47">
+        <v>30</v>
+      </c>
+      <c r="R27" s="17" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C28" s="20" t="s">
         <v>212</v>
       </c>
@@ -50536,8 +50779,14 @@
         <v>222</v>
       </c>
       <c r="N28" s="22"/>
-    </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q28" s="47">
+        <v>31</v>
+      </c>
+      <c r="R28" s="17" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C29" s="20" t="s">
         <v>212</v>
       </c>
@@ -50559,8 +50808,14 @@
         <v>227</v>
       </c>
       <c r="N29" s="22"/>
-    </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q29" s="47">
+        <v>32</v>
+      </c>
+      <c r="R29" s="17" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C30" s="20" t="s">
         <v>212</v>
       </c>
@@ -50582,8 +50837,14 @@
         <v>232</v>
       </c>
       <c r="N30" s="22"/>
-    </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q30" s="47">
+        <v>33</v>
+      </c>
+      <c r="R30" s="17" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C31" s="20" t="s">
         <v>233</v>
       </c>
@@ -50605,8 +50866,14 @@
         <v>238</v>
       </c>
       <c r="N31" s="22"/>
-    </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q31" s="47">
+        <v>34</v>
+      </c>
+      <c r="R31" s="17" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C32" s="20" t="s">
         <v>239</v>
       </c>
@@ -50628,8 +50895,14 @@
         <v>244</v>
       </c>
       <c r="N32" s="22"/>
-    </row>
-    <row r="33" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q32" s="47">
+        <v>35</v>
+      </c>
+      <c r="R32" s="17" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="33" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C33" s="20" t="s">
         <v>239</v>
       </c>
@@ -50651,8 +50924,14 @@
         <v>249</v>
       </c>
       <c r="N33" s="22"/>
-    </row>
-    <row r="34" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q33" s="47">
+        <v>36</v>
+      </c>
+      <c r="R33" s="17" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="34" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C34" s="20" t="s">
         <v>250</v>
       </c>
@@ -50674,8 +50953,14 @@
         <v>255</v>
       </c>
       <c r="N34" s="22"/>
-    </row>
-    <row r="35" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q34" s="47">
+        <v>37</v>
+      </c>
+      <c r="R34" s="17" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="35" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C35" s="20" t="s">
         <v>250</v>
       </c>
@@ -50697,8 +50982,14 @@
         <v>260</v>
       </c>
       <c r="N35" s="22"/>
-    </row>
-    <row r="36" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q35" s="47">
+        <v>38</v>
+      </c>
+      <c r="R35" s="17" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="36" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C36" s="20" t="s">
         <v>250</v>
       </c>
@@ -50720,8 +51011,14 @@
         <v>264</v>
       </c>
       <c r="N36" s="22"/>
-    </row>
-    <row r="37" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q36" s="47">
+        <v>39</v>
+      </c>
+      <c r="R36" s="17" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="37" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C37" s="20" t="s">
         <v>250</v>
       </c>
@@ -50743,8 +51040,14 @@
         <v>268</v>
       </c>
       <c r="N37" s="22"/>
-    </row>
-    <row r="38" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q37" s="47">
+        <v>40</v>
+      </c>
+      <c r="R37" s="17" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="38" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C38" s="20" t="s">
         <v>269</v>
       </c>
@@ -50766,8 +51069,14 @@
         <v>273</v>
       </c>
       <c r="N38" s="22"/>
-    </row>
-    <row r="39" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q38" s="47">
+        <v>41</v>
+      </c>
+      <c r="R38" s="17" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="39" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C39" s="20" t="s">
         <v>269</v>
       </c>
@@ -50789,8 +51098,14 @@
         <v>278</v>
       </c>
       <c r="N39" s="22"/>
-    </row>
-    <row r="40" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q39" s="47">
+        <v>42</v>
+      </c>
+      <c r="R39" s="17" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="40" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C40" s="20" t="s">
         <v>269</v>
       </c>
@@ -50812,8 +51127,14 @@
         <v>283</v>
       </c>
       <c r="N40" s="22"/>
-    </row>
-    <row r="41" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q40" s="47">
+        <v>43</v>
+      </c>
+      <c r="R40" s="17" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="41" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C41" s="20" t="s">
         <v>269</v>
       </c>
@@ -50835,8 +51156,14 @@
         <v>288</v>
       </c>
       <c r="N41" s="22"/>
-    </row>
-    <row r="42" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q41" s="47">
+        <v>44</v>
+      </c>
+      <c r="R41" s="17" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="42" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C42" s="20" t="s">
         <v>269</v>
       </c>
@@ -50858,8 +51185,14 @@
         <v>293</v>
       </c>
       <c r="N42" s="22"/>
-    </row>
-    <row r="43" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q42" s="47">
+        <v>45</v>
+      </c>
+      <c r="R42" s="17" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="43" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C43" s="20" t="s">
         <v>269</v>
       </c>
@@ -50881,8 +51214,14 @@
         <v>298</v>
       </c>
       <c r="N43" s="22"/>
-    </row>
-    <row r="44" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q43" s="47">
+        <v>46</v>
+      </c>
+      <c r="R43" s="17" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="44" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C44" s="20" t="s">
         <v>269</v>
       </c>
@@ -50904,8 +51243,14 @@
         <v>303</v>
       </c>
       <c r="N44" s="22"/>
-    </row>
-    <row r="45" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q44" s="47">
+        <v>47</v>
+      </c>
+      <c r="R44" s="17" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="45" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C45" s="20" t="s">
         <v>269</v>
       </c>
@@ -50927,8 +51272,14 @@
         <v>307</v>
       </c>
       <c r="N45" s="22"/>
-    </row>
-    <row r="46" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q45" s="47">
+        <v>48</v>
+      </c>
+      <c r="R45" s="17" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="46" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C46" s="20" t="s">
         <v>269</v>
       </c>
@@ -50950,8 +51301,14 @@
         <v>312</v>
       </c>
       <c r="N46" s="22"/>
-    </row>
-    <row r="47" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q46" s="47">
+        <v>49</v>
+      </c>
+      <c r="R46" s="17" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="47" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C47" s="20" t="s">
         <v>269</v>
       </c>
@@ -50973,8 +51330,14 @@
         <v>317</v>
       </c>
       <c r="N47" s="22"/>
-    </row>
-    <row r="48" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q47" s="47">
+        <v>50</v>
+      </c>
+      <c r="R47" s="17" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="48" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C48" s="20" t="s">
         <v>269</v>
       </c>
@@ -50996,8 +51359,14 @@
         <v>322</v>
       </c>
       <c r="N48" s="22"/>
-    </row>
-    <row r="49" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q48" s="47">
+        <v>51</v>
+      </c>
+      <c r="R48" s="17" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="49" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C49" s="20" t="s">
         <v>323</v>
       </c>
@@ -51019,8 +51388,14 @@
         <v>328</v>
       </c>
       <c r="N49" s="22"/>
-    </row>
-    <row r="50" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q49" s="47">
+        <v>52</v>
+      </c>
+      <c r="R49" s="17" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="50" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C50" s="20" t="s">
         <v>323</v>
       </c>
@@ -51042,8 +51417,14 @@
         <v>333</v>
       </c>
       <c r="N50" s="22"/>
-    </row>
-    <row r="51" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q50" s="47">
+        <v>53</v>
+      </c>
+      <c r="R50" s="17" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="51" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C51" s="20" t="s">
         <v>323</v>
       </c>
@@ -51065,8 +51446,14 @@
         <v>338</v>
       </c>
       <c r="N51" s="22"/>
-    </row>
-    <row r="52" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q51" s="47">
+        <v>54</v>
+      </c>
+      <c r="R51" s="17" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="52" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C52" s="20" t="s">
         <v>323</v>
       </c>
@@ -51088,8 +51475,14 @@
         <v>343</v>
       </c>
       <c r="N52" s="22"/>
-    </row>
-    <row r="53" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q52" s="47">
+        <v>55</v>
+      </c>
+      <c r="R52" s="17" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="53" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C53" s="20" t="s">
         <v>323</v>
       </c>
@@ -51111,8 +51504,14 @@
         <v>348</v>
       </c>
       <c r="N53" s="22"/>
-    </row>
-    <row r="54" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q53" s="47">
+        <v>56</v>
+      </c>
+      <c r="R53" s="17" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="54" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C54" s="20" t="s">
         <v>323</v>
       </c>
@@ -51134,8 +51533,14 @@
         <v>353</v>
       </c>
       <c r="N54" s="22"/>
-    </row>
-    <row r="55" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q54" s="47">
+        <v>57</v>
+      </c>
+      <c r="R54" s="17" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="55" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C55" s="20" t="s">
         <v>354</v>
       </c>
@@ -51157,8 +51562,14 @@
         <v>359</v>
       </c>
       <c r="N55" s="22"/>
-    </row>
-    <row r="56" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="Q55" s="47">
+        <v>58</v>
+      </c>
+      <c r="R55" s="48" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="56" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C56" s="20" t="s">
         <v>354</v>
       </c>
@@ -51181,7 +51592,7 @@
       </c>
       <c r="N56" s="22"/>
     </row>
-    <row r="57" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C57" s="20" t="s">
         <v>365</v>
       </c>
@@ -51204,7 +51615,7 @@
       </c>
       <c r="N57" s="22"/>
     </row>
-    <row r="58" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C58" s="20" t="s">
         <v>371</v>
       </c>
@@ -51227,7 +51638,7 @@
       </c>
       <c r="N58" s="22"/>
     </row>
-    <row r="59" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C59" s="20" t="s">
         <v>377</v>
       </c>
@@ -51250,7 +51661,7 @@
       </c>
       <c r="N59" s="22"/>
     </row>
-    <row r="60" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C60" s="20" t="s">
         <v>383</v>
       </c>
@@ -51273,7 +51684,7 @@
       </c>
       <c r="N60" s="22"/>
     </row>
-    <row r="61" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C61" s="20" t="s">
         <v>389</v>
       </c>
@@ -51296,7 +51707,7 @@
       </c>
       <c r="N61" s="22"/>
     </row>
-    <row r="62" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C62" s="20" t="s">
         <v>395</v>
       </c>
@@ -51319,7 +51730,7 @@
       </c>
       <c r="N62" s="22"/>
     </row>
-    <row r="63" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C63" s="20" t="s">
         <v>395</v>
       </c>
@@ -51342,7 +51753,7 @@
       </c>
       <c r="N63" s="22"/>
     </row>
-    <row r="64" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C64" s="20" t="s">
         <v>395</v>
       </c>
@@ -53434,5 +53845,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>